<commit_message>
update empty test template
</commit_message>
<xml_diff>
--- a/tox5_preprocessing/src/TOX5/test_data/hts_metadata_tmp/TestDataRecordingForm_harmless_HTS_METADATA_empty.xlsx
+++ b/tox5_preprocessing/src/TOX5/test_data/hts_metadata_tmp/TestDataRecordingForm_harmless_HTS_METADATA_empty.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8325" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8325" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -2722,8 +2722,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="36" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="36"/>
+    <col min="1" max="5" width="8.85546875" style="36" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14.45" customHeight="1">
@@ -3109,8 +3109,8 @@
     <col min="8" max="8" width="5.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.85546875" style="36" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="22" width="8.85546875" style="36" customWidth="1"/>
-    <col min="23" max="16384" width="8.85546875" style="36"/>
+    <col min="12" max="24" width="8.85546875" style="36" customWidth="1"/>
+    <col min="25" max="16384" width="8.85546875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -5493,8 +5493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5505,8 +5505,8 @@
     <col min="4" max="4" width="16.28515625" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="36" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68" style="36" customWidth="1"/>
-    <col min="7" max="17" width="8.85546875" style="36" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="36"/>
+    <col min="7" max="19" width="8.85546875" style="36" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5699,7 +5699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K2"/>
     </sheetView>
   </sheetViews>
@@ -5710,8 +5710,8 @@
     <col min="3" max="6" width="8.85546875" style="17" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="17" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" style="17" customWidth="1"/>
-    <col min="9" max="11" width="8.85546875" style="17" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="17"/>
+    <col min="9" max="13" width="8.85546875" style="17" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="39.6" customHeight="1">

</xml_diff>